<commit_message>
Allow early retirement of capacity in Services
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_FT_Demands.xlsx
+++ b/SuppXLS/Scen_SYS_FT_Demands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37517DD8-E90D-4533-8CD4-8CC9536C6205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB04D3C-5BAE-427C-AB5F-B15795847B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="7" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="200">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -664,6 +664,24 @@
   </si>
   <si>
     <t>*0</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>RCAP_BND</t>
+  </si>
+  <si>
+    <t>S-*</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>CAP_BND</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -2024,7 +2042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
@@ -2146,7 +2164,7 @@
   <dimension ref="B1:AC455"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38957,10 +38975,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B650A31E-B81F-4A4F-9C3A-301ECD552AAC}">
-  <dimension ref="B2:F5"/>
+  <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38970,12 +38988,12 @@
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -38994,7 +39012,7 @@
         <v>National</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>70</v>
       </c>
@@ -39008,7 +39026,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>72</v>
       </c>
@@ -39020,6 +39038,84 @@
       </c>
       <c r="F5" t="s">
         <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="3" t="str">
+        <f>Regions!C3</f>
+        <v>IE</v>
+      </c>
+      <c r="F9" s="3" t="str">
+        <f>Regions!D3</f>
+        <v>National</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introduce CAP_BND and early retirement for industry and residential
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_FT_Demands.xlsx
+++ b/SuppXLS/Scen_SYS_FT_Demands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB04D3C-5BAE-427C-AB5F-B15795847B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FCD09C-35A2-4B23-9D47-C864DB1A3D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="199">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -670,9 +670,6 @@
   </si>
   <si>
     <t>RCAP_BND</t>
-  </si>
-  <si>
-    <t>S-*</t>
   </si>
   <si>
     <t>~TFM_INS</t>
@@ -38978,7 +38975,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39042,7 +39039,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -39064,7 +39061,7 @@
         <v>National</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -39075,7 +39072,7 @@
         <v>195</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -39086,10 +39083,10 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -39103,10 +39100,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="E12">
         <v>5</v>

</xml_diff>